<commit_message>
update em 2021 excel file; layout changes
</commit_message>
<xml_diff>
--- a/src/excel_templates/EM_2021.xlsx
+++ b/src/excel_templates/EM_2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev_sync\1_Github\fredbet\src\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CB2B3B-9B4A-4101-8730-462D4D526927}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A2EB44-EF91-433B-8D01-D2388AAFE5BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="240">
   <si>
     <t>Country 1</t>
   </si>
@@ -449,9 +449,6 @@
     <t>FINLAND</t>
   </si>
   <si>
-    <t>FYR_MACEDONIA</t>
-  </si>
-  <si>
     <t>GEORGIA</t>
   </si>
   <si>
@@ -725,40 +722,31 @@
     <t>Kopenhagen</t>
   </si>
   <si>
-    <t>Play-off D</t>
-  </si>
-  <si>
     <t>Amsterdam</t>
   </si>
   <si>
     <t>Bukarest</t>
   </si>
   <si>
-    <t>Play-off C</t>
-  </si>
-  <si>
     <t>London</t>
   </si>
   <si>
     <t>Glasgow</t>
   </si>
   <si>
-    <t>Play-off B</t>
-  </si>
-  <si>
     <t>Bilbao</t>
   </si>
   <si>
     <t>Dublin</t>
   </si>
   <si>
-    <t>Play-off A</t>
-  </si>
-  <si>
     <t>München</t>
   </si>
   <si>
     <t>Budapest</t>
+  </si>
+  <si>
+    <t>MACEDONIA</t>
   </si>
 </sst>
 </file>
@@ -1128,7 +1116,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E440"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1167,10 +1157,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="2">
-        <v>43994.875</v>
+        <v>44358.875</v>
       </c>
       <c r="E2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1184,10 +1174,10 @@
         <v>7</v>
       </c>
       <c r="D3" s="2">
-        <v>43995.625</v>
+        <v>44359.625</v>
       </c>
       <c r="E3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1201,10 +1191,10 @@
         <v>7</v>
       </c>
       <c r="D4" s="2">
-        <v>43999.875</v>
+        <v>44363.875</v>
       </c>
       <c r="E4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1218,10 +1208,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="2">
-        <v>43999.75</v>
+        <v>44363.75</v>
       </c>
       <c r="E5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1235,10 +1225,10 @@
         <v>7</v>
       </c>
       <c r="D6" s="2">
-        <v>44003.75</v>
+        <v>44367.75</v>
       </c>
       <c r="E6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1252,10 +1242,10 @@
         <v>7</v>
       </c>
       <c r="D7" s="2">
-        <v>44003.75</v>
+        <v>44367.75</v>
       </c>
       <c r="E7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1266,13 +1256,13 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D8" s="2">
-        <v>43995.875</v>
+        <v>44359.875</v>
       </c>
       <c r="E8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1283,13 +1273,13 @@
         <v>139</v>
       </c>
       <c r="C9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D9" s="2">
-        <v>43995.75</v>
+        <v>44359.75</v>
       </c>
       <c r="E9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1300,13 +1290,13 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D10" s="2">
-        <v>43999.625</v>
+        <v>44363.625</v>
       </c>
       <c r="E10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1317,13 +1307,13 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D11" s="2">
-        <v>44000.75</v>
+        <v>44364.75</v>
       </c>
       <c r="E11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1334,13 +1324,13 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D12" s="2">
-        <v>44004.875</v>
+        <v>44368.875</v>
       </c>
       <c r="E12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1351,30 +1341,30 @@
         <v>136</v>
       </c>
       <c r="C13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D13" s="2">
-        <v>44004.875</v>
+        <v>44368.875</v>
       </c>
       <c r="E13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D14" s="2">
-        <v>43996.875</v>
+        <v>44360.875</v>
       </c>
       <c r="E14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1382,33 +1372,33 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
+        <v>239</v>
+      </c>
+      <c r="C15" t="s">
+        <v>216</v>
+      </c>
+      <c r="D15" s="2">
+        <v>44360.75</v>
+      </c>
+      <c r="E15" t="s">
         <v>232</v>
-      </c>
-      <c r="C15" t="s">
-        <v>217</v>
-      </c>
-      <c r="D15" s="2">
-        <v>43996.75</v>
-      </c>
-      <c r="E15" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D16" s="2">
-        <v>44000.875</v>
+        <v>44364.875</v>
       </c>
       <c r="E16" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1416,33 +1406,33 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
+        <v>239</v>
+      </c>
+      <c r="C17" t="s">
+        <v>216</v>
+      </c>
+      <c r="D17" s="2">
+        <v>44364.625</v>
+      </c>
+      <c r="E17" t="s">
         <v>232</v>
-      </c>
-      <c r="C17" t="s">
-        <v>217</v>
-      </c>
-      <c r="D17" s="2">
-        <v>44000.625</v>
-      </c>
-      <c r="E17" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="B18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D18" s="2">
-        <v>44004.75</v>
+        <v>44368.75</v>
       </c>
       <c r="E18" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1453,13 +1443,13 @@
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D19" s="2">
-        <v>44004.75</v>
+        <v>44368.75</v>
       </c>
       <c r="E19" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1470,30 +1460,30 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D20" s="2">
-        <v>43996.625</v>
+        <v>44360.625</v>
       </c>
       <c r="E20" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>235</v>
+        <v>156</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D21" s="2">
-        <v>43997.625</v>
+        <v>44361.625</v>
       </c>
       <c r="E21" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1501,16 +1491,16 @@
         <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>235</v>
+        <v>156</v>
       </c>
       <c r="C22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D22" s="2">
-        <v>44001.875</v>
+        <v>44365.875</v>
       </c>
       <c r="E22" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1521,13 +1511,13 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D23" s="2">
-        <v>44001.75</v>
+        <v>44365.75</v>
       </c>
       <c r="E23" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1538,13 +1528,13 @@
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D24" s="2">
-        <v>44005.875</v>
+        <v>44369.875</v>
       </c>
       <c r="E24" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1552,16 +1542,16 @@
         <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>235</v>
+        <v>156</v>
       </c>
       <c r="C25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D25" s="2">
-        <v>44005.875</v>
+        <v>44369.875</v>
       </c>
       <c r="E25" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1572,13 +1562,13 @@
         <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D26" s="2">
-        <v>43997.875</v>
+        <v>44361.875</v>
       </c>
       <c r="E26" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1586,16 +1576,16 @@
         <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>238</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D27" s="2">
-        <v>43997.75</v>
+        <v>44361.75</v>
       </c>
       <c r="E27" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1603,16 +1593,16 @@
         <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>238</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D28" s="2">
-        <v>44001.625</v>
+        <v>44365.625</v>
       </c>
       <c r="E28" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1623,30 +1613,30 @@
         <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D29" s="2">
-        <v>44002.875</v>
+        <v>44366.875</v>
       </c>
       <c r="E29" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>238</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
         <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D30" s="2">
-        <v>44006.75</v>
+        <v>44370.75</v>
       </c>
       <c r="E30" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1657,13 +1647,13 @@
         <v>17</v>
       </c>
       <c r="C31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D31" s="2">
-        <v>44006.75</v>
+        <v>44370.75</v>
       </c>
       <c r="E31" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1674,30 +1664,30 @@
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D32" s="2">
-        <v>43998.875</v>
+        <v>44362.875</v>
       </c>
       <c r="E32" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>241</v>
+        <v>28</v>
       </c>
       <c r="B33" t="s">
         <v>18</v>
       </c>
       <c r="C33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D33" s="2">
-        <v>43998.75</v>
+        <v>44362.75</v>
       </c>
       <c r="E33" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1708,30 +1698,30 @@
         <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D34" s="2">
-        <v>44002.75</v>
+        <v>44366.75</v>
       </c>
       <c r="E34" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>241</v>
+        <v>28</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D35" s="2">
-        <v>44002.625</v>
+        <v>44366.625</v>
       </c>
       <c r="E35" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1739,16 +1729,16 @@
         <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>241</v>
+        <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D36" s="2">
-        <v>44006.875</v>
+        <v>44370.875</v>
       </c>
       <c r="E36" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1759,13 +1749,13 @@
         <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D37" s="2">
-        <v>44006.875</v>
+        <v>44370.875</v>
       </c>
       <c r="E37" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3006,8 +2996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A210"/>
   <sheetViews>
-    <sheetView topLeftCell="A191" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3032,7 +3022,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -3047,17 +3037,17 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
@@ -3067,7 +3057,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -3087,7 +3077,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
@@ -3102,7 +3092,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -3117,7 +3107,7 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
@@ -3127,7 +3117,7 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
@@ -3137,7 +3127,7 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
@@ -3152,12 +3142,12 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
@@ -3192,7 +3182,7 @@
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
@@ -3202,7 +3192,7 @@
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
@@ -3217,7 +3207,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -3232,7 +3222,7 @@
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
@@ -3252,12 +3242,12 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
@@ -3267,12 +3257,12 @@
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
@@ -3297,17 +3287,17 @@
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
@@ -3317,7 +3307,7 @@
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
@@ -3352,7 +3342,7 @@
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
@@ -3367,32 +3357,32 @@
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>140</v>
+        <v>42</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>141</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>44</v>
+        <v>141</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
@@ -3402,37 +3392,37 @@
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>143</v>
+        <v>175</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>176</v>
+        <v>93</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>176</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>177</v>
+        <v>45</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>46</v>
+        <v>177</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
@@ -3447,137 +3437,137 @@
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>180</v>
+        <v>94</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>11</v>
+        <v>143</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>144</v>
+        <v>13</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>40</v>
+        <v>180</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>181</v>
+        <v>98</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>99</v>
+        <v>144</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>145</v>
+        <v>56</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>56</v>
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>101</v>
+        <v>145</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>146</v>
+        <v>102</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>104</v>
+        <v>146</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>147</v>
+        <v>105</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>105</v>
+        <v>57</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>59</v>
+        <v>147</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
@@ -3592,12 +3582,12 @@
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>150</v>
+        <v>106</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>106</v>
+        <v>239</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
@@ -3627,7 +3617,7 @@
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
@@ -3642,12 +3632,12 @@
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
@@ -3657,12 +3647,12 @@
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
@@ -3692,22 +3682,22 @@
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
@@ -3727,7 +3717,7 @@
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
@@ -3747,22 +3737,22 @@
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
@@ -3782,7 +3772,7 @@
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
@@ -3807,12 +3797,12 @@
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
@@ -3827,7 +3817,7 @@
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
@@ -3837,7 +3827,7 @@
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
@@ -3862,12 +3852,12 @@
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
@@ -3897,17 +3887,17 @@
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
@@ -3917,7 +3907,7 @@
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
@@ -3942,7 +3932,7 @@
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
@@ -3972,12 +3962,12 @@
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
@@ -3997,7 +3987,7 @@
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
@@ -4017,17 +4007,17 @@
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
@@ -4037,12 +4027,12 @@
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
@@ -4067,7 +4057,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A210">
-    <sortCondition ref="A1"/>
+    <sortCondition ref="A1:A210"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4093,62 +4083,62 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>